<commit_message>
add test 9 10. Not analyse yet
</commit_message>
<xml_diff>
--- a/Others/TestCuts/5TestCut2MIP2/Result/pre_cut2.xlsx
+++ b/Others/TestCuts/5TestCut2MIP2/Result/pre_cut2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\PFE\MyWork\PFE\Others\TestCuts\TestCut2MIP2\Result\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\PFE\MyWork\PFE\Others\TestCuts\5TestCut2MIP2\Result\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2675,7 +2675,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2861,6 +2861,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -3022,9 +3046,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3349,10 +3379,10 @@
   <dimension ref="A1:Z161"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D113" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="J107" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J1" sqref="J1:J1048576"/>
+      <selection pane="bottomRight" activeCell="W113" sqref="W113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3362,7 +3392,10 @@
     <col min="5" max="5" width="0.28515625" customWidth="1"/>
     <col min="6" max="8" width="9.140625" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="9.140625" customWidth="1"/>
-    <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="0.140625" customWidth="1"/>
+    <col min="11" max="12" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="1.28515625" hidden="1" customWidth="1"/>
+    <col min="14" max="22" width="9.140625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -8312,7 +8345,7 @@
       <c r="V62" t="s">
         <v>254</v>
       </c>
-      <c r="W62" t="s">
+      <c r="W62" s="2" t="s">
         <v>259</v>
       </c>
       <c r="X62">
@@ -8392,7 +8425,7 @@
       <c r="V63" t="s">
         <v>261</v>
       </c>
-      <c r="W63" t="s">
+      <c r="W63" s="2" t="s">
         <v>265</v>
       </c>
       <c r="X63">
@@ -8472,7 +8505,7 @@
       <c r="V64" t="s">
         <v>267</v>
       </c>
-      <c r="W64" t="s">
+      <c r="W64" s="2" t="s">
         <v>272</v>
       </c>
       <c r="X64">
@@ -8712,7 +8745,7 @@
       <c r="V67" t="s">
         <v>286</v>
       </c>
-      <c r="W67" t="s">
+      <c r="W67" s="6" t="s">
         <v>290</v>
       </c>
       <c r="X67">
@@ -9032,7 +9065,7 @@
       <c r="V71" t="s">
         <v>310</v>
       </c>
-      <c r="W71" t="s">
+      <c r="W71" s="2" t="s">
         <v>314</v>
       </c>
       <c r="X71">
@@ -9592,7 +9625,7 @@
       <c r="V78" t="s">
         <v>351</v>
       </c>
-      <c r="W78" t="s">
+      <c r="W78" s="2" t="s">
         <v>355</v>
       </c>
       <c r="X78">
@@ -9752,7 +9785,7 @@
       <c r="V80" t="s">
         <v>362</v>
       </c>
-      <c r="W80" t="s">
+      <c r="W80" s="7" t="s">
         <v>366</v>
       </c>
       <c r="X80">
@@ -10152,7 +10185,7 @@
       <c r="V85" t="s">
         <v>394</v>
       </c>
-      <c r="W85" t="s">
+      <c r="W85" s="2" t="s">
         <v>398</v>
       </c>
       <c r="X85">
@@ -10232,7 +10265,7 @@
       <c r="V86" t="s">
         <v>400</v>
       </c>
-      <c r="W86" t="s">
+      <c r="W86" s="2" t="s">
         <v>403</v>
       </c>
       <c r="X86">
@@ -10472,7 +10505,7 @@
       <c r="V89" t="s">
         <v>419</v>
       </c>
-      <c r="W89" t="s">
+      <c r="W89" s="4" t="s">
         <v>423</v>
       </c>
       <c r="X89">
@@ -10632,7 +10665,7 @@
       <c r="V91" t="s">
         <v>435</v>
       </c>
-      <c r="W91" t="s">
+      <c r="W91" s="4" t="s">
         <v>436</v>
       </c>
       <c r="X91">
@@ -10792,7 +10825,7 @@
       <c r="V93" t="s">
         <v>445</v>
       </c>
-      <c r="W93" t="s">
+      <c r="W93" s="5" t="s">
         <v>448</v>
       </c>
       <c r="X93">
@@ -10872,7 +10905,7 @@
       <c r="V94" t="s">
         <v>450</v>
       </c>
-      <c r="W94" t="s">
+      <c r="W94" s="2" t="s">
         <v>453</v>
       </c>
       <c r="X94">
@@ -11112,7 +11145,7 @@
       <c r="V97" t="s">
         <v>462</v>
       </c>
-      <c r="W97" t="s">
+      <c r="W97" s="2" t="s">
         <v>465</v>
       </c>
       <c r="X97">
@@ -11272,7 +11305,7 @@
       <c r="V99" t="s">
         <v>474</v>
       </c>
-      <c r="W99" t="s">
+      <c r="W99" s="2" t="s">
         <v>478</v>
       </c>
       <c r="X99">
@@ -11592,7 +11625,7 @@
       <c r="V103" t="s">
         <v>488</v>
       </c>
-      <c r="W103" t="s">
+      <c r="W103" s="4" t="s">
         <v>489</v>
       </c>
       <c r="X103">
@@ -11912,7 +11945,7 @@
       <c r="V107" t="s">
         <v>507</v>
       </c>
-      <c r="W107" t="s">
+      <c r="W107" s="2" t="s">
         <v>512</v>
       </c>
       <c r="X107">
@@ -12072,7 +12105,7 @@
       <c r="V109" t="s">
         <v>526</v>
       </c>
-      <c r="W109" t="s">
+      <c r="W109" s="3" t="s">
         <v>527</v>
       </c>
       <c r="X109">
@@ -12312,7 +12345,7 @@
       <c r="V112" t="s">
         <v>543</v>
       </c>
-      <c r="W112" t="s">
+      <c r="W112" s="2" t="s">
         <v>547</v>
       </c>
       <c r="X112">
@@ -12392,7 +12425,7 @@
       <c r="V113" t="s">
         <v>549</v>
       </c>
-      <c r="W113" t="s">
+      <c r="W113" s="2" t="s">
         <v>554</v>
       </c>
       <c r="X113">
@@ -12872,7 +12905,7 @@
       <c r="V119" t="s">
         <v>591</v>
       </c>
-      <c r="W119" t="s">
+      <c r="W119" s="2" t="s">
         <v>595</v>
       </c>
       <c r="X119">
@@ -13032,7 +13065,7 @@
       <c r="V121" t="s">
         <v>604</v>
       </c>
-      <c r="W121" t="s">
+      <c r="W121" s="2" t="s">
         <v>608</v>
       </c>
       <c r="X121">
@@ -16247,5 +16280,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add test18. See list of changes for other updates
</commit_message>
<xml_diff>
--- a/Others/TestCuts/5TestCut2MIP2/Result/pre_cut2.xlsx
+++ b/Others/TestCuts/5TestCut2MIP2/Result/pre_cut2.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="pre_cut2" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -3379,19 +3379,20 @@
   <dimension ref="A1:Z161"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="J107" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W113" sqref="W113"/>
+      <selection pane="bottomRight" activeCell="W1" activeCellId="1" sqref="A1:B1048576 W1:W1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
-    <col min="5" max="5" width="0.28515625" customWidth="1"/>
-    <col min="6" max="8" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="9.140625" customWidth="1"/>
     <col min="10" max="10" width="0.140625" customWidth="1"/>
     <col min="11" max="12" width="9.140625" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="1.28515625" hidden="1" customWidth="1"/>

</xml_diff>